<commit_message>
Improved handling of ICScards number formats.
</commit_message>
<xml_diff>
--- a/testdata/source/icscards/icscards_big.xlsx
+++ b/testdata/source/icscards/icscards_big.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\beancount-import\testdata\source\icscards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA72930-2794-45A2-9E0F-492A1EC261D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D13099B-255A-466E-AA61-4D4080C9AD5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1573,9 +1573,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$EGP]\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$ZAR]\ #,##0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1647,7 +1649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1678,17 +1680,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1697,22 +1717,26 @@
       <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
@@ -1726,33 +1750,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2245,7 +2253,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2266,118 +2274,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="31" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
     </row>
     <row r="2" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
     </row>
     <row r="6" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="15">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="21">
         <v>500</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
       <c r="L6" s="5" t="s">
         <v>9</v>
       </c>
@@ -2386,22 +2394,22 @@
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="15">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="21">
         <v>500</v>
       </c>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
       <c r="L7" s="5" t="s">
         <v>9</v>
       </c>
@@ -2410,63 +2418,63 @@
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="15">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="21">
         <v>500</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
       <c r="L8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="35" t="s">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="11"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="6"/>
       <c r="K10" s="4">
         <v>7.99</v>
@@ -2479,22 +2487,22 @@
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="11"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="6"/>
       <c r="K11" s="4">
         <v>89.9</v>
@@ -2507,23 +2515,23 @@
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="7" t="s">
+      <c r="I12" s="15"/>
+      <c r="J12" s="36" t="s">
         <v>25</v>
       </c>
       <c r="K12" s="4">
@@ -2535,18 +2543,18 @@
     </row>
     <row r="13" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="11" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="8">
         <v>19.882400000000001</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -2555,23 +2563,23 @@
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="7" t="s">
+      <c r="I14" s="15"/>
+      <c r="J14" s="37" t="s">
         <v>31</v>
       </c>
       <c r="K14" s="4">
@@ -2583,18 +2591,18 @@
     </row>
     <row r="15" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="11" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="8">
         <v>16.12903</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -2603,22 +2611,22 @@
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="11"/>
+      <c r="I16" s="15"/>
       <c r="J16" s="7" t="s">
         <v>36</v>
       </c>
@@ -2631,18 +2639,18 @@
     </row>
     <row r="17" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="11" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="8">
         <v>15.942629999999999</v>
       </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -2651,22 +2659,22 @@
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="11"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="7" t="s">
         <v>39</v>
       </c>
@@ -2679,18 +2687,18 @@
     </row>
     <row r="19" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="11" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="8">
         <v>16.132010000000001</v>
       </c>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -2699,22 +2707,22 @@
       <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="11"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="7" t="s">
         <v>43</v>
       </c>
@@ -2727,18 +2735,18 @@
     </row>
     <row r="21" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="11" t="s">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="8">
         <v>16.134450000000001</v>
       </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -2747,22 +2755,22 @@
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11" t="s">
+      <c r="C22" s="15"/>
+      <c r="D22" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
       <c r="G22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="11"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="7" t="s">
         <v>44</v>
       </c>
@@ -2775,18 +2783,18 @@
     </row>
     <row r="23" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="11" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
       <c r="G23" s="8">
         <v>16.135079999999999</v>
       </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -2795,22 +2803,22 @@
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
       <c r="G24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="11"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="7" t="s">
         <v>48</v>
       </c>
@@ -2823,18 +2831,18 @@
     </row>
     <row r="25" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="11" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
       <c r="G25" s="8">
         <v>16.046209999999999</v>
       </c>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
@@ -2843,22 +2851,22 @@
       <c r="A26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="15"/>
+      <c r="D26" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
       <c r="G26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I26" s="11"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="6"/>
       <c r="K26" s="4">
         <v>26.33</v>
@@ -2871,22 +2879,22 @@
       <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="11"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="7" t="s">
         <v>51</v>
       </c>
@@ -2899,18 +2907,18 @@
     </row>
     <row r="28" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="11" t="s">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
       <c r="G28" s="8">
         <v>16.12903</v>
       </c>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
@@ -2919,22 +2927,22 @@
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
       <c r="G29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I29" s="11"/>
+      <c r="I29" s="15"/>
       <c r="J29" s="7" t="s">
         <v>54</v>
       </c>
@@ -2947,24 +2955,24 @@
     </row>
     <row r="30" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="11" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
       <c r="G30" s="8">
         <v>16.04682</v>
       </c>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:13" ht="31.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="16" t="s">
         <v>131</v>
       </c>
       <c r="B31" s="17"/>
@@ -2998,44 +3006,123 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
     </row>
     <row r="34" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
     </row>
     <row r="35" spans="1:13" ht="408.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:13" ht="408.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="86">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="H29:I29"/>
     <mergeCell ref="A33:M33"/>
     <mergeCell ref="A34:M34"/>
     <mergeCell ref="B30:C30"/>
@@ -3043,91 +3130,13 @@
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="A31:M31"/>
     <mergeCell ref="A32:M32"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A9:M9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:M4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A34" r:id="rId1" display="http://www.icscards.nl/depositogarantiestelsel" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3159,226 +3168,226 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="33" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="22" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+      <c r="A2" s="31">
         <v>43482</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32">
         <v>99999999999</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32">
         <v>1</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="25" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
     </row>
     <row r="3" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="10" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="26" t="s">
+      <c r="I3" s="19"/>
+      <c r="J3" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
     </row>
     <row r="5" spans="1:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="21" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="11" t="s">
+      <c r="H5" s="27"/>
+      <c r="I5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="21">
         <v>8.7200000000000006</v>
       </c>
-      <c r="M5" s="15"/>
+      <c r="M5" s="21"/>
       <c r="N5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="11" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="27">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="28">
         <v>16.055050000000001</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="21" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="11" t="s">
+      <c r="H7" s="27"/>
+      <c r="I7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="21">
         <v>172.36</v>
       </c>
-      <c r="M7" s="15"/>
+      <c r="M7" s="21"/>
       <c r="N7" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="11" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="27">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="28">
         <v>16.134830000000001</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
       <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="21" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="11" t="s">
+      <c r="H9" s="27"/>
+      <c r="I9" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="11"/>
+      <c r="J9" s="15"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="15">
+      <c r="L9" s="21">
         <v>35.96</v>
       </c>
-      <c r="M9" s="15"/>
+      <c r="M9" s="21"/>
       <c r="N9" s="5" t="s">
         <v>17</v>
       </c>
@@ -3387,392 +3396,392 @@
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="21" t="s">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="11" t="s">
+      <c r="H10" s="27"/>
+      <c r="I10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="11"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="21">
         <v>32.72</v>
       </c>
-      <c r="M10" s="15"/>
+      <c r="M10" s="21"/>
       <c r="N10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="11" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="27">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="28">
         <v>16.04523</v>
       </c>
-      <c r="H11" s="27"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
       <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="21" t="s">
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="11" t="s">
+      <c r="H12" s="27"/>
+      <c r="I12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="11"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="21">
         <v>15.58</v>
       </c>
-      <c r="M12" s="15"/>
+      <c r="M12" s="21"/>
       <c r="N12" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="11" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="27">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="28">
         <v>16.046209999999999</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
       <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="21" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="11" t="s">
+      <c r="H14" s="27"/>
+      <c r="I14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="11"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="21">
         <v>77.900000000000006</v>
       </c>
-      <c r="M14" s="15"/>
+      <c r="M14" s="21"/>
       <c r="N14" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="11" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="27">
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="28">
         <v>16.046209999999999</v>
       </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
       <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="21" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="11" t="s">
+      <c r="H16" s="27"/>
+      <c r="I16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="11"/>
+      <c r="J16" s="15"/>
       <c r="K16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="21">
         <v>26.01</v>
       </c>
-      <c r="M16" s="15"/>
+      <c r="M16" s="21"/>
       <c r="N16" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="11" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="27">
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="28">
         <v>16.147639999999999</v>
       </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
       <c r="N17" s="6"/>
     </row>
     <row r="18" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="21" t="s">
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="11" t="s">
+      <c r="H18" s="27"/>
+      <c r="I18" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="11"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L18" s="15">
+      <c r="L18" s="21">
         <v>14.65</v>
       </c>
-      <c r="M18" s="15"/>
+      <c r="M18" s="21"/>
       <c r="N18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="11" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="27">
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="28">
         <v>16.040959999999998</v>
       </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
       <c r="K19" s="6"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
       <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="21" t="s">
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="11" t="s">
+      <c r="H20" s="27"/>
+      <c r="I20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="11"/>
+      <c r="J20" s="15"/>
       <c r="K20" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L20" s="21">
         <v>13.09</v>
       </c>
-      <c r="M20" s="15"/>
+      <c r="M20" s="21"/>
       <c r="N20" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="11" t="s">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="27">
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="28">
         <v>16.04278</v>
       </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
       <c r="N21" s="6"/>
     </row>
     <row r="22" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11" t="s">
+      <c r="C22" s="15"/>
+      <c r="D22" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="21" t="s">
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="11" t="s">
+      <c r="H22" s="27"/>
+      <c r="I22" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="11"/>
+      <c r="J22" s="15"/>
       <c r="K22" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="L22" s="15">
+      <c r="L22" s="21">
         <v>34.270000000000003</v>
       </c>
-      <c r="M22" s="15"/>
+      <c r="M22" s="21"/>
       <c r="N22" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="11" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="27">
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="28">
         <v>16.049019999999999</v>
       </c>
-      <c r="H23" s="27"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
       <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="21" t="s">
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="11" t="s">
+      <c r="H24" s="27"/>
+      <c r="I24" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="11"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="6"/>
-      <c r="L24" s="15">
+      <c r="L24" s="21">
         <v>193.1</v>
       </c>
-      <c r="M24" s="15"/>
+      <c r="M24" s="21"/>
       <c r="N24" s="5" t="s">
         <v>17</v>
       </c>
@@ -3781,340 +3790,340 @@
       <c r="A25" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11" t="s">
+      <c r="C25" s="15"/>
+      <c r="D25" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="21" t="s">
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="11" t="s">
+      <c r="H25" s="27"/>
+      <c r="I25" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J25" s="11"/>
+      <c r="J25" s="15"/>
       <c r="K25" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="L25" s="15">
+      <c r="L25" s="21">
         <v>24.26</v>
       </c>
-      <c r="M25" s="15"/>
+      <c r="M25" s="21"/>
       <c r="N25" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="11" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="27">
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="28">
         <v>16.075849999999999</v>
       </c>
-      <c r="H26" s="27"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
       <c r="K26" s="6"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
       <c r="N26" s="6"/>
     </row>
     <row r="27" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="21" t="s">
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="11" t="s">
+      <c r="H27" s="27"/>
+      <c r="I27" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J27" s="11"/>
+      <c r="J27" s="15"/>
       <c r="K27" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="L27" s="15">
+      <c r="L27" s="21">
         <v>14.31</v>
       </c>
-      <c r="M27" s="15"/>
+      <c r="M27" s="21"/>
       <c r="N27" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="11" t="s">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="27">
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="28">
         <v>16.072679999999998</v>
       </c>
-      <c r="H28" s="27"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
       <c r="N28" s="6"/>
     </row>
     <row r="29" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="21" t="s">
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="11" t="s">
+      <c r="H29" s="27"/>
+      <c r="I29" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="11"/>
+      <c r="J29" s="15"/>
       <c r="K29" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="L29" s="15">
+      <c r="L29" s="21">
         <v>14.93</v>
       </c>
-      <c r="M29" s="15"/>
+      <c r="M29" s="21"/>
       <c r="N29" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="11" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="27">
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="28">
         <v>16.075019999999999</v>
       </c>
-      <c r="H30" s="27"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
       <c r="N30" s="6"/>
     </row>
     <row r="31" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11" t="s">
+      <c r="C31" s="15"/>
+      <c r="D31" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="21" t="s">
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="11" t="s">
+      <c r="H31" s="27"/>
+      <c r="I31" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="11"/>
+      <c r="J31" s="15"/>
       <c r="K31" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="L31" s="15">
+      <c r="L31" s="21">
         <v>30.68</v>
       </c>
-      <c r="M31" s="15"/>
+      <c r="M31" s="21"/>
       <c r="N31" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="11" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="27">
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="28">
         <v>16.07236</v>
       </c>
-      <c r="H32" s="27"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
       <c r="K32" s="6"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
       <c r="N32" s="6"/>
     </row>
     <row r="33" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11" t="s">
+      <c r="C33" s="15"/>
+      <c r="D33" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="21" t="s">
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="11" t="s">
+      <c r="H33" s="27"/>
+      <c r="I33" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="11"/>
+      <c r="J33" s="15"/>
       <c r="K33" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="L33" s="15">
+      <c r="L33" s="21">
         <v>140.01</v>
       </c>
-      <c r="M33" s="15"/>
+      <c r="M33" s="21"/>
       <c r="N33" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="11" t="s">
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="27">
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="28">
         <v>16.07028</v>
       </c>
-      <c r="H34" s="27"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
       <c r="K34" s="6"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
       <c r="N34" s="6"/>
     </row>
     <row r="35" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11" t="s">
+      <c r="C35" s="15"/>
+      <c r="D35" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="21" t="s">
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="H35" s="21"/>
-      <c r="I35" s="11" t="s">
+      <c r="H35" s="27"/>
+      <c r="I35" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="11"/>
+      <c r="J35" s="15"/>
       <c r="K35" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="L35" s="15">
+      <c r="L35" s="21">
         <v>62.49</v>
       </c>
-      <c r="M35" s="15"/>
+      <c r="M35" s="21"/>
       <c r="N35" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="11" t="s">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="27">
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="28">
         <v>16.002559999999999</v>
       </c>
-      <c r="H36" s="27"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
       <c r="K36" s="6"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
       <c r="N36" s="6"/>
     </row>
     <row r="37" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="21" t="s">
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="H37" s="21"/>
-      <c r="I37" s="11" t="s">
+      <c r="H37" s="27"/>
+      <c r="I37" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="J37" s="11"/>
+      <c r="J37" s="15"/>
       <c r="K37" s="6"/>
-      <c r="L37" s="15">
+      <c r="L37" s="21">
         <v>55</v>
       </c>
-      <c r="M37" s="15"/>
+      <c r="M37" s="21"/>
       <c r="N37" s="5" t="s">
         <v>17</v>
       </c>
@@ -4123,104 +4132,104 @@
       <c r="A38" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11" t="s">
+      <c r="C38" s="15"/>
+      <c r="D38" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="21" t="s">
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="H38" s="21"/>
-      <c r="I38" s="11" t="s">
+      <c r="H38" s="27"/>
+      <c r="I38" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J38" s="11"/>
+      <c r="J38" s="15"/>
       <c r="K38" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="L38" s="15">
+      <c r="L38" s="21">
         <v>17.97</v>
       </c>
-      <c r="M38" s="15"/>
+      <c r="M38" s="21"/>
       <c r="N38" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="11" t="s">
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="27">
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="28">
         <v>15.581519999999999</v>
       </c>
-      <c r="H39" s="27"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
       <c r="K39" s="6"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
       <c r="N39" s="6"/>
     </row>
     <row r="40" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11" t="s">
+      <c r="C40" s="15"/>
+      <c r="D40" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="21" t="s">
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="H40" s="21"/>
-      <c r="I40" s="11" t="s">
+      <c r="H40" s="27"/>
+      <c r="I40" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J40" s="11"/>
+      <c r="J40" s="15"/>
       <c r="K40" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="L40" s="15">
+      <c r="L40" s="21">
         <v>52.62</v>
       </c>
-      <c r="M40" s="15"/>
+      <c r="M40" s="21"/>
       <c r="N40" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="11" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="27">
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="28">
         <v>15.58343</v>
       </c>
-      <c r="H41" s="27"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
       <c r="K41" s="6"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="16"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
       <c r="N41" s="6"/>
     </row>
     <row r="42" spans="1:14" ht="408.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4228,195 +4237,6 @@
     <row r="44" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="201">
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:K4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="L5:M5"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
@@ -4429,6 +4249,195 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="L41:M41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -4465,129 +4474,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="33" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="22" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
       <c r="M1" s="6"/>
     </row>
     <row r="2" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+      <c r="A2" s="31">
         <v>43482</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32">
         <v>99999999999</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32">
         <v>1</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="25" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="10" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="19"/>
+      <c r="J3" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
       <c r="M3" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
     </row>
     <row r="5" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="22" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="18" t="s">
         <v>115</v>
       </c>
       <c r="J5" s="18"/>
-      <c r="K5" s="15">
+      <c r="K5" s="21">
         <v>96</v>
       </c>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
       <c r="O5" s="5" t="s">
         <v>17</v>
       </c>
@@ -4596,29 +4605,29 @@
       <c r="A6" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="22" t="s">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="30"/>
       <c r="I6" s="18" t="s">
         <v>115</v>
       </c>
       <c r="J6" s="18"/>
-      <c r="K6" s="15">
+      <c r="K6" s="21">
         <v>94</v>
       </c>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
       <c r="O6" s="5" t="s">
         <v>17</v>
       </c>
@@ -4627,29 +4636,29 @@
       <c r="A7" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="22" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="18" t="s">
         <v>115</v>
       </c>
       <c r="J7" s="18"/>
-      <c r="K7" s="15">
+      <c r="K7" s="21">
         <v>49</v>
       </c>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
       <c r="O7" s="5" t="s">
         <v>17</v>
       </c>
@@ -4664,21 +4673,14 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
@@ -4687,14 +4689,21 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:K4"/>
     <mergeCell ref="L4:P4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>